<commit_message>
New and improved data
</commit_message>
<xml_diff>
--- a/output_file/June HighLow/example.xlsx
+++ b/output_file/June HighLow/example.xlsx
@@ -404,10 +404,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>9.9390261415366033E-7</v>
+        <v>8.1136674085319101E-7</v>
       </c>
       <c r="D2">
-        <v>8.2295278490908022E-6</v>
+        <v>3.7509935931492223E-6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -418,10 +418,10 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1.7479040755233455E-7</v>
+        <v>3.3666975575769974E-7</v>
       </c>
       <c r="D3">
-        <v>4.3529476959103844E-6</v>
+        <v>5.093179931801366E-6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -432,10 +432,10 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>4.6674320758529177E-7</v>
+        <v>2.9579641935961374E-7</v>
       </c>
       <c r="D4">
-        <v>3.8085215761420614E-6</v>
+        <v>4.434911698039949E-6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -446,10 +446,10 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>7.8709170433707467E-7</v>
+        <v>7.6673044799612167E-7</v>
       </c>
       <c r="D5">
-        <v>9.568988608052408E-6</v>
+        <v>9.7982132643955486E-6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -460,10 +460,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>6.1545056799556813E-7</v>
+        <v>3.0389655735927201E-7</v>
       </c>
       <c r="D6">
-        <v>9.279920890481894E-6</v>
+        <v>8.661728199638102E-6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -474,10 +474,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>6.5123214425081549E-7</v>
+        <v>2.8364068158047258E-7</v>
       </c>
       <c r="D7">
-        <v>4.6373461749732108E-6</v>
+        <v>1.4274051761355427E-6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -488,10 +488,10 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1.6760909060333443E-7</v>
+        <v>1.1569222546407478E-7</v>
       </c>
       <c r="D8">
-        <v>1.4607365343098426E-6</v>
+        <v>1.3260625935398497E-6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,10 +502,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>4.6313848155418973E-7</v>
+        <v>3.6743012105145298E-7</v>
       </c>
       <c r="D9">
-        <v>5.9060388663728317E-6</v>
+        <v>6.1221772250674309E-6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,10 +516,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>4.3281237426534165E-7</v>
+        <v>4.297830925690078E-7</v>
       </c>
       <c r="D10">
-        <v>4.5736926705412276E-6</v>
+        <v>4.0425304004628967E-6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,10 +530,10 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>7.8047924456351384E-7</v>
+        <v>6.4583945350743678E-7</v>
       </c>
       <c r="D11">
-        <v>2.6463353339950635E-6</v>
+        <v>2.3211322811561626E-6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,10 +544,10 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>1.6807977653907873E-7</v>
+        <v>2.7261069379320483E-7</v>
       </c>
       <c r="D12">
-        <v>1.6419817004633927E-6</v>
+        <v>2.1986276846215571E-6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,10 +558,10 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>8.4976191297304266E-7</v>
+        <v>8.3538025681897459E-7</v>
       </c>
       <c r="D13">
-        <v>3.4668661039456849E-6</v>
+        <v>2.516521103209655E-6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>4.0864073591864376E-7</v>
+        <v>5.287181452069531E-7</v>
       </c>
       <c r="D14">
-        <v>4.3444636910384182E-6</v>
+        <v>4.5152058757573658E-6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,10 +586,10 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>3.7740691593664371E-7</v>
+        <v>6.0415301002292821E-7</v>
       </c>
       <c r="D15">
-        <v>8.365137507033221E-6</v>
+        <v>8.1415948129031797E-6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -600,10 +600,10 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>5.8480277631290266E-7</v>
+        <v>8.057576638837652E-7</v>
       </c>
       <c r="D16">
-        <v>3.390276512204231E-6</v>
+        <v>5.0886599312374179E-6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,10 +614,10 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>1.5129140211336311E-7</v>
+        <v>1.1255726700897765E-7</v>
       </c>
       <c r="D17">
-        <v>2.4176120913129383E-6</v>
+        <v>1.2316956061026578E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>